<commit_message>
fix sample data (error in months
</commit_message>
<xml_diff>
--- a/sample_data/listado_pacientes.xlsx
+++ b/sample_data/listado_pacientes.xlsx
@@ -502,36 +502,36 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Lucila Lourdes Aller Lillo</t>
+          <t>Cloe Mercader Pera</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>19046</v>
+        <v>13548</v>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>14665734Z</t>
+          <t>24542949V</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>699234346</v>
+        <v>620108348</v>
       </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Glorieta de Anselma Guitart 519
-Soria, 07099</t>
+          <t>C. Marita Pujadas 10
+Jaén, 42052</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>ciprianomolina@yahoo.com</t>
+          <t>hugocanovas@yahoo.com</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Psicologo3</t>
+          <t>Elena</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -540,40 +540,40 @@
         </is>
       </c>
       <c r="K2" s="2" t="n">
-        <v>41446</v>
+        <v>16345</v>
       </c>
       <c r="L2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Rosendo Iglesias</t>
+          <t>Máximo Agustí Galiano</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>33137</v>
+        <v>31127</v>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>56683053J</t>
+          <t>96746138L</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>644268972</v>
+        <v>601327677</v>
       </c>
       <c r="F3" t="n">
-        <v>645133057</v>
+        <v>652893194</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Urbanización de José Ángel Morata 54
-Santa Cruz de Tenerife, 15703</t>
+          <t>Rambla de Flavia Otero 77
+Granada, 37337</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>bertapombo@gmail.com</t>
+          <t>odalysquevedo@hotmail.com</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -587,49 +587,47 @@
         </is>
       </c>
       <c r="K3" s="2" t="n">
-        <v>31346</v>
+        <v>22319</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Actor</t>
+          <t>Profesional de medicina alternativa</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Claudio Casemiro Herranz Echeverría</t>
+          <t>Juliana Amalia Luís Cerro</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>27565</v>
+        <v>5639</v>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>20121384H</t>
+          <t>65416954D</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>626127369</v>
-      </c>
-      <c r="F4" t="n">
-        <v>635817854</v>
-      </c>
+        <v>673079480</v>
+      </c>
+      <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Ronda Salud Girona 75 Apt. 46 
-La Rioja, 49676</t>
+          <t>Rambla de Horacio Girón 57 Puerta 6 
+Soria, 07776</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>wdieguez@hotmail.com</t>
+          <t>jose-angelzabala@hotmail.com</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Elena</t>
+          <t>Psicologo3</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -638,46 +636,38 @@
         </is>
       </c>
       <c r="K4" s="2" t="n">
-        <v>33277</v>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>Técnico en ciencias biológicas</t>
-        </is>
-      </c>
+        <v>18234</v>
+      </c>
+      <c r="L4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Rosario del Sarmiento</t>
+          <t>Lola Conesa Agustí</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>39233</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Wilfredo del Gomila</t>
-        </is>
-      </c>
+        <v>7526</v>
+      </c>
+      <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>70491670M</t>
+          <t>92116835H</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>690722981</v>
+        <v>647530889</v>
       </c>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Cañada de Gisela Beltran 93
-Ciudad, 17934</t>
+          <t>Avenida Arcelia Ordóñez 276
+Melilla, 32974</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>lermaclaudia@yahoo.com</t>
+          <t>nataliocobos@hotmail.com</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -691,38 +681,40 @@
         </is>
       </c>
       <c r="K5" s="2" t="n">
-        <v>27018</v>
+        <v>37511</v>
       </c>
       <c r="L5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Chucho Pallarès-Patiño</t>
+          <t>Serafina Hernandez Blanch</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>27220</v>
+        <v>29161</v>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>75675820R</t>
+          <t>49144449G</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>665470525</v>
-      </c>
-      <c r="F6" t="inlineStr"/>
+        <v>603837270</v>
+      </c>
+      <c r="F6" t="n">
+        <v>697918385</v>
+      </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Cuesta Amaya Pintor 25 Piso 3 
-Alicante, 45174</t>
+          <t>Vial de Marcio Casares 166
+La Rioja, 19332</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>pedrazagabino@hotmail.com</t>
+          <t>curro84@gmail.com</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -736,45 +728,49 @@
         </is>
       </c>
       <c r="K6" s="2" t="n">
-        <v>36054</v>
-      </c>
-      <c r="L6" t="inlineStr"/>
+        <v>22907</v>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Técnico en aparatos de diagnóstico y tratamiento médico</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Vidal Barros Lillo</t>
+          <t>Osvaldo Nogués Palacios</t>
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>7261</v>
+        <v>27157</v>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>79783301G</t>
+          <t>33841962S</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>682931771</v>
+        <v>614952390</v>
       </c>
       <c r="F7" t="n">
-        <v>674538833</v>
+        <v>649549202</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Rambla de Nereida Tejedor 562 Puerta 7 
-Huelva, 13495</t>
+          <t>Calle de Serafina Llanos 4
+Burgos, 46605</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>ividal@gmail.com</t>
+          <t>vicenteadadia@hotmail.com</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Psicologo3</t>
+          <t>Oriol</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -783,42 +779,44 @@
         </is>
       </c>
       <c r="K7" s="2" t="n">
-        <v>8471</v>
+        <v>2836</v>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Moldeador y machero</t>
+          <t>Compositor</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Nicanor Ojeda Haro</t>
+          <t>Agustina Vélez Blázquez</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>13920</v>
+        <v>35263</v>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>16548172V</t>
+          <t>80825285L</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>614388117</v>
-      </c>
-      <c r="F8" t="inlineStr"/>
+        <v>666341079</v>
+      </c>
+      <c r="F8" t="n">
+        <v>669667855</v>
+      </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Avenida Quique Cepeda 4 Puerta 9 
-Tarragona, 48153</t>
+          <t>Camino de Araceli Alegria 88
+Sevilla, 04254</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>jesus67@yahoo.com</t>
+          <t>kcoronado@yahoo.com</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -832,49 +830,47 @@
         </is>
       </c>
       <c r="K8" s="2" t="n">
-        <v>24768</v>
-      </c>
-      <c r="L8" t="inlineStr"/>
+        <v>32237</v>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Deportista</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Marcos Borja González</t>
+          <t>Cristian Carbajo Hernandez</t>
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>40736</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Aitor del Mir</t>
-        </is>
-      </c>
+        <v>32731</v>
+      </c>
+      <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>60196888T</t>
+          <t>25820527Z</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>616527111</v>
-      </c>
-      <c r="F9" t="n">
-        <v>679116126</v>
-      </c>
+        <v>604199947</v>
+      </c>
+      <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Calle Epifanio Ibañez 594 Puerta 3 
-La Coruña, 10701</t>
+          <t>Callejón Édgar Calderón 65 Piso 5 
+Vizcaya, 10707</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>ncastello@gmail.com</t>
+          <t>anitavergara@yahoo.com</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Elena</t>
+          <t>Psicologo3</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -883,42 +879,38 @@
         </is>
       </c>
       <c r="K9" s="2" t="n">
-        <v>24288</v>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>Personal de limpieza</t>
-        </is>
-      </c>
+        <v>22672</v>
+      </c>
+      <c r="L9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Josep del Mosquera</t>
+          <t>Maximiano Canals-Aramburu</t>
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>8100</v>
+        <v>12198</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
-          <t>83974519R</t>
+          <t>15318660Q</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>600169101</v>
+        <v>670341450</v>
       </c>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Vial de Juan Carlos Calderon 19 Piso 8 
-Santa Cruz de Tenerife, 24400</t>
+          <t>Pasaje de Cornelio Cuesta 3
+Soria, 02873</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>carnerotelmo@yahoo.com</t>
+          <t>custodiolaguna@yahoo.com</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -932,47 +924,43 @@
         </is>
       </c>
       <c r="K10" s="2" t="n">
-        <v>11809</v>
+        <v>28165</v>
       </c>
       <c r="L10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Lucila Elodia Cabo Vigil</t>
+          <t>Ciriaco de Acosta</t>
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>42042</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Bienvenida de Briones</t>
-        </is>
-      </c>
+        <v>22178</v>
+      </c>
+      <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
-          <t>77018110B</t>
+          <t>74962378L</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>688132038</v>
+        <v>651793753</v>
       </c>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Ronda Celestino Jover 263 Piso 4 
-Segovia, 20778</t>
+          <t>Cañada de Dorita Villegas 51
+Burgos, 03277</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>edmundopalma@hotmail.com</t>
+          <t>joan25@yahoo.com</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Elena</t>
+          <t>Oriol</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -981,7 +969,7 @@
         </is>
       </c>
       <c r="K11" s="2" t="n">
-        <v>2460</v>
+        <v>7173</v>
       </c>
       <c r="L11" t="inlineStr"/>
     </row>

</xml_diff>